<commit_message>
add neutrons final pictures
</commit_message>
<xml_diff>
--- a/neutrons/e(V_0).xlsx
+++ b/neutrons/e(V_0).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,19 +467,19 @@
         <v>18</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C4" si="0">A3/$K$2*600</f>
+        <f t="shared" ref="C3" si="0">A3/$K$2*600</f>
         <v>13.432835820895521</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D4" si="1">C3 / (1.8 + 0.4 / $J$2)</f>
+        <f t="shared" ref="D3" si="1">C3 / (1.8 + 0.4 / $J$2)</f>
         <v>6.5269264960464133</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E4" si="2">D3/$J$2</f>
+        <f t="shared" ref="E3:E5" si="2">D3/$J$2</f>
         <v>4.2109203200299437</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F4" si="3">(A3/$K$2*40) / 1.6</f>
+        <f t="shared" ref="F3" si="3">(A3/$K$2*40) / 1.6</f>
         <v>0.55970149253731338</v>
       </c>
     </row>
@@ -488,11 +488,11 @@
         <v>20</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="0"/>
+        <f>A4/$K$2*600</f>
         <v>14.925373134328359</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="1"/>
+        <f>C4 / (1.8 + 0.4 / $J$2)</f>
         <v>7.2521405511626824</v>
       </c>
       <c r="E4" s="1">
@@ -500,8 +500,29 @@
         <v>4.6788003555888276</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="3"/>
+        <f>(A4/$K$2*40) / 1.6</f>
         <v>0.62189054726368154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>13.7</v>
+      </c>
+      <c r="C5" s="1">
+        <f>A5/$K$2*600</f>
+        <v>10.223880597014926</v>
+      </c>
+      <c r="D5" s="1">
+        <f>C5 / (1.8 + 0.4 / $J$2)</f>
+        <v>4.9677162775464376</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="2"/>
+        <v>3.2049782435783469</v>
+      </c>
+      <c r="F5" s="1">
+        <f>(A5/$K$2*40) / 1.6</f>
+        <v>0.42599502487562185</v>
       </c>
     </row>
   </sheetData>
@@ -514,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>